<commit_message>
Final changes before repository hand-in
</commit_message>
<xml_diff>
--- a/Outputs/Table 1 A.xlsx
+++ b/Outputs/Table 1 A.xlsx
@@ -112,19 +112,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1.2038562395428602E8</v>
+        <v>8.532630061677904E7</v>
       </c>
       <c r="C2" t="n">
-        <v>1.319856516726155E8</v>
+        <v>9.906888723512885E7</v>
       </c>
       <c r="D2" t="n">
-        <v>1.4358567939094514E8</v>
+        <v>1.128114738534783E8</v>
       </c>
       <c r="E2" t="n">
-        <v>1.5518570710927466E8</v>
+        <v>1.2655406047182785E8</v>
       </c>
       <c r="F2" t="n">
-        <v>1.6678573482760426E8</v>
+        <v>1.4029664709017748E8</v>
       </c>
     </row>
     <row r="3">
@@ -132,19 +132,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>1.4070465459200194E8</v>
+        <v>1.9821675583586156E8</v>
       </c>
       <c r="C3" t="n">
-        <v>1.5230468231033143E8</v>
+        <v>2.1195934245421135E8</v>
       </c>
       <c r="D3" t="n">
-        <v>1.6390471002866104E8</v>
+        <v>2.2570192907256082E8</v>
       </c>
       <c r="E3" t="n">
-        <v>1.7550473774699062E8</v>
+        <v>2.3944451569091037E8</v>
       </c>
       <c r="F3" t="n">
-        <v>1.8710476546532017E8</v>
+        <v>2.5318710230926E8</v>
       </c>
     </row>
     <row r="4">
@@ -152,19 +152,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>1.8135541067105237E8</v>
+        <v>4.2423482604219234E8</v>
       </c>
       <c r="C4" t="n">
-        <v>1.929554383893819E8</v>
+        <v>4.3797741266054213E8</v>
       </c>
       <c r="D4" t="n">
-        <v>2.0455546610771152E8</v>
+        <v>4.5171999927889156E8</v>
       </c>
       <c r="E4" t="n">
-        <v>2.1615549382604104E8</v>
+        <v>4.654625858972412E8</v>
       </c>
       <c r="F4" t="n">
-        <v>2.2775552154437062E8</v>
+        <v>4.7920517251559085E8</v>
       </c>
     </row>
     <row r="5">
@@ -172,19 +172,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>2.301586696450917E8</v>
+        <v>6.958744244650055E8</v>
       </c>
       <c r="C5" t="n">
-        <v>2.417586973634212E8</v>
+        <v>7.096170110833554E8</v>
       </c>
       <c r="D5" t="n">
-        <v>2.5335872508175084E8</v>
+        <v>7.233595977017049E8</v>
       </c>
       <c r="E5" t="n">
-        <v>2.649587528000804E8</v>
+        <v>7.371021843200544E8</v>
       </c>
       <c r="F5" t="n">
-        <v>2.765587805184099E8</v>
+        <v>7.50844770938404E8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made final changes before sending to collabs
</commit_message>
<xml_diff>
--- a/Outputs/Table 1 A.xlsx
+++ b/Outputs/Table 1 A.xlsx
@@ -112,19 +112,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>1.4429877187442875E8</v>
+        <v>1.441354900088777E8</v>
       </c>
       <c r="C2" t="n">
-        <v>1.623272035651798E8</v>
+        <v>1.6216392169962877E8</v>
       </c>
       <c r="D2" t="n">
-        <v>1.8035563525593108E8</v>
+        <v>1.8019235339038002E8</v>
       </c>
       <c r="E2" t="n">
-        <v>1.9838406694668207E8</v>
+        <v>1.9822078508113098E8</v>
       </c>
       <c r="F2" t="n">
-        <v>2.1641249863743365E8</v>
+        <v>2.1624921677188253E8</v>
       </c>
     </row>
     <row r="3">
@@ -132,19 +132,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="n">
-        <v>2.5878762012374258E8</v>
+        <v>2.5846095045082933E8</v>
       </c>
       <c r="C3" t="n">
-        <v>2.7681605181449366E8</v>
+        <v>2.7648938214158034E8</v>
       </c>
       <c r="D3" t="n">
-        <v>2.948444835052449E8</v>
+        <v>2.945178138323316E8</v>
       </c>
       <c r="E3" t="n">
-        <v>3.1287291519599587E8</v>
+        <v>3.125462455230826E8</v>
       </c>
       <c r="F3" t="n">
-        <v>3.309013468867475E8</v>
+        <v>3.3057467721383417E8</v>
       </c>
     </row>
     <row r="4">
@@ -152,19 +152,19 @@
         <v>7</v>
       </c>
       <c r="B4" t="n">
-        <v>4.880056224446769E8</v>
+        <v>4.873518590557416E8</v>
       </c>
       <c r="C4" t="n">
-        <v>5.0603405413542783E8</v>
+        <v>5.053802907464927E8</v>
       </c>
       <c r="D4" t="n">
-        <v>5.2406248582617915E8</v>
+        <v>5.2340872243724394E8</v>
       </c>
       <c r="E4" t="n">
-        <v>5.420909175169301E8</v>
+        <v>5.414371541279949E8</v>
       </c>
       <c r="F4" t="n">
-        <v>5.601193492076817E8</v>
+        <v>5.594655858187464E8</v>
       </c>
     </row>
     <row r="5">
@@ -172,19 +172,19 @@
         <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>7.634906829992691E8</v>
+        <v>7.624438466366886E8</v>
       </c>
       <c r="C5" t="n">
-        <v>7.815191146900202E8</v>
+        <v>7.804722783274397E8</v>
       </c>
       <c r="D5" t="n">
-        <v>7.995475463807715E8</v>
+        <v>7.985007100181911E8</v>
       </c>
       <c r="E5" t="n">
-        <v>8.175759780715225E8</v>
+        <v>8.16529141708942E8</v>
       </c>
       <c r="F5" t="n">
-        <v>8.356044097622739E8</v>
+        <v>8.345575733996935E8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>